<commit_message>
Update location of fluence and count staticstics
</commit_message>
<xml_diff>
--- a/results/Cs137/Cs137_R_30_cm_Nr_2000000000_ISO_model_det1_det2_det3 - Unfolded Fluence Spectrum.xlsx
+++ b/results/Cs137/Cs137_R_30_cm_Nr_2000000000_ISO_model_det1_det2_det3 - Unfolded Fluence Spectrum.xlsx
@@ -520,31 +520,31 @@
         <v>0.01982943797740053</v>
       </c>
       <c r="F2" t="n">
-        <v>9.824651690452342</v>
+        <v>9.82461274400216</v>
       </c>
       <c r="G2" t="n">
-        <v>9.62492178399936</v>
+        <v>9.6226578296356</v>
       </c>
       <c r="H2" t="n">
-        <v>10.0265113792361</v>
+        <v>10.03087779307675</v>
       </c>
       <c r="I2" t="n">
-        <v>0.002527242653168935</v>
+        <v>0.002528852152208033</v>
       </c>
       <c r="J2" t="n">
-        <v>0.002245492202227781</v>
+        <v>0.002253088948055081</v>
       </c>
       <c r="K2" t="n">
-        <v>0.002854528859736951</v>
+        <v>0.002861120764638966</v>
       </c>
       <c r="L2" t="n">
-        <v>0.008890363398223938</v>
+        <v>0.008890180060885326</v>
       </c>
       <c r="M2" t="n">
-        <v>0.00869479618168984</v>
+        <v>0.008697326742682056</v>
       </c>
       <c r="N2" t="n">
-        <v>0.009089729607002456</v>
+        <v>0.009091865758660951</v>
       </c>
     </row>
     <row r="3">
@@ -566,31 +566,31 @@
         <v>0.0499839736740351</v>
       </c>
       <c r="F3" t="n">
-        <v>0.04664501539242744</v>
+        <v>0.04664534464428318</v>
       </c>
       <c r="G3" t="n">
-        <v>0.04635438174126001</v>
+        <v>0.04634631039237534</v>
       </c>
       <c r="H3" t="n">
-        <v>0.04693971001269212</v>
+        <v>0.0469325087099207</v>
       </c>
       <c r="I3" t="n">
-        <v>0.04508521895389653</v>
+        <v>0.04508553840610342</v>
       </c>
       <c r="J3" t="n">
-        <v>0.04480532918421806</v>
+        <v>0.04479752780671629</v>
       </c>
       <c r="K3" t="n">
-        <v>0.04536802261305288</v>
+        <v>0.04536103108637986</v>
       </c>
       <c r="L3" t="n">
-        <v>0.04669551756735525</v>
+        <v>0.04669584838478093</v>
       </c>
       <c r="M3" t="n">
-        <v>0.04640491492797095</v>
+        <v>0.04639689118820508</v>
       </c>
       <c r="N3" t="n">
-        <v>0.04699022364357902</v>
+        <v>0.04698308668758529</v>
       </c>
     </row>
     <row r="4">
@@ -612,31 +612,31 @@
         <v>0.06981341165143562</v>
       </c>
       <c r="F4" t="n">
-        <v>9.87129670584477</v>
+        <v>9.871258088646442</v>
       </c>
       <c r="G4" t="n">
-        <v>9.67127616574062</v>
+        <v>9.669004140027974</v>
       </c>
       <c r="H4" t="n">
-        <v>10.0734510892488</v>
+        <v>10.07781030178667</v>
       </c>
       <c r="I4" t="n">
-        <v>0.04761246160706547</v>
+        <v>0.04761439055831146</v>
       </c>
       <c r="J4" t="n">
-        <v>0.04705082138644583</v>
+        <v>0.04705061675477137</v>
       </c>
       <c r="K4" t="n">
-        <v>0.04822255147278982</v>
+        <v>0.04822215185101883</v>
       </c>
       <c r="L4" t="n">
-        <v>0.05558588096557919</v>
+        <v>0.05558602844566626</v>
       </c>
       <c r="M4" t="n">
-        <v>0.05509971110966079</v>
+        <v>0.05509421793088713</v>
       </c>
       <c r="N4" t="n">
-        <v>0.05607995325058147</v>
+        <v>0.05607495244624622</v>
       </c>
     </row>
   </sheetData>

</xml_diff>